<commit_message>
Latest information model spreadsheets from Jay.
</commit_message>
<xml_diff>
--- a/resources/FHIM_dbp_refSetMapping.xlsx
+++ b/resources/FHIM_dbp_refSetMapping.xlsx
@@ -7,15 +7,16 @@
     <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" tabRatio="758"/>
   </bookViews>
   <sheets>
-    <sheet name="source" sheetId="1" r:id="rId1"/>
-    <sheet name="FHIMObservationRefSet" sheetId="2" r:id="rId2"/>
-    <sheet name="FHIMObservationCodeRefSet" sheetId="3" r:id="rId3"/>
-    <sheet name="AltFHIMObservationCodeRefSet" sheetId="6" r:id="rId4"/>
-    <sheet name="FHIMObservationDataRefSet" sheetId="5" r:id="rId5"/>
-    <sheet name="FHIMObservationCompRefSet" sheetId="4" r:id="rId6"/>
-    <sheet name="FHIMObservationConstraintRefSet" sheetId="7" r:id="rId7"/>
+    <sheet name="Questions" sheetId="8" r:id="rId1"/>
+    <sheet name="source" sheetId="1" r:id="rId2"/>
+    <sheet name="FHIMObservationRefSet" sheetId="2" r:id="rId3"/>
+    <sheet name="FHIMObservationCodeRefSet" sheetId="3" r:id="rId4"/>
+    <sheet name="AltFHIMObservationCodeRefSet" sheetId="6" r:id="rId5"/>
+    <sheet name="FHIMObservationDataRefSet" sheetId="5" r:id="rId6"/>
+    <sheet name="FHIMObservationCompRefSet" sheetId="4" r:id="rId7"/>
+    <sheet name="FHIMObservationConstraintRefSet" sheetId="7" r:id="rId8"/>
   </sheets>
-  <calcPr calcId="125725"/>
+  <calcPr calcId="125725" concurrentCalc="0"/>
 </workbook>
 </file>
 
@@ -275,26 +276,12 @@
         </r>
       </text>
     </comment>
-    <comment ref="B13" authorId="0">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>temporarily using name, but will be an SCT CID</t>
-        </r>
-      </text>
-    </comment>
   </commentList>
 </comments>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="185" uniqueCount="97">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="190" uniqueCount="103">
   <si>
     <t>DiastolicBloodPressureObservation</t>
   </si>
@@ -347,9 +334,6 @@
     <t>reliability</t>
   </si>
   <si>
-    <t>severity</t>
-  </si>
-  <si>
     <t>status</t>
   </si>
   <si>
@@ -488,9 +472,6 @@
     <t>Reliability</t>
   </si>
   <si>
-    <t>Severity</t>
-  </si>
-  <si>
     <t>Status</t>
   </si>
   <si>
@@ -506,9 +487,6 @@
     <t xml:space="preserve">memberID for Reliability in DiastolicBloodPressureObservation </t>
   </si>
   <si>
-    <t xml:space="preserve">memberID for Severity in DiastolicBloodPressureObservation </t>
-  </si>
-  <si>
     <t xml:space="preserve">memberID for Status in DiastolicBloodPressureObservation </t>
   </si>
   <si>
@@ -585,13 +563,63 @@
   </si>
   <si>
     <t>componentId for Provenance in FHIMObservationComposition</t>
+  </si>
+  <si>
+    <t>#</t>
+  </si>
+  <si>
+    <t>Are there any criteria for refset type selection--i.e., whether to include more columns in fewer refsets or fewer columns in more refsets?</t>
+  </si>
+  <si>
+    <t>In the base model refset, a concept ID is associated with a type. Why is this? Is it in order to differentiate different model types (FHIM, CEM) for the same concept?</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">In the CEM key refset, an IMHC key code is associated with the concept identifier. Wouldn't that key code </t>
+    </r>
+    <r>
+      <rPr>
+        <u/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>be</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> the concept identifier?</t>
+    </r>
+  </si>
+  <si>
+    <t>In the FHIM key refset, should the LOINC code be a CID, assuming it's in the workbench environment, or do we need to specify its system and text?</t>
+  </si>
+  <si>
+    <t>Do we want to classify components as CEM does, if the source model does not?</t>
+  </si>
+  <si>
+    <t>Constraints use a property called "path," which seems to be a description of the kind of constraint, but which I'd expect to be a concept rather than a string.</t>
+  </si>
+  <si>
+    <t>I've asserted some constraint criteria as value set OIDs. Does that fit in this conceptual solution?</t>
+  </si>
+  <si>
+    <t>Question</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="3">
+  <fonts count="4">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -613,6 +641,14 @@
       <color indexed="81"/>
       <name val="Tahoma"/>
       <family val="2"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="2">
@@ -653,16 +689,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>6</xdr:col>
-      <xdr:colOff>285750</xdr:colOff>
-      <xdr:row>8</xdr:row>
-      <xdr:rowOff>180975</xdr:rowOff>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>247650</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>9525</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>10</xdr:col>
-      <xdr:colOff>38100</xdr:colOff>
-      <xdr:row>33</xdr:row>
-      <xdr:rowOff>38100</xdr:rowOff>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>4381500</xdr:colOff>
+      <xdr:row>27</xdr:row>
+      <xdr:rowOff>57150</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -680,7 +716,7 @@
       </xdr:blipFill>
       <xdr:spPr bwMode="auto">
         <a:xfrm>
-          <a:off x="7353300" y="1704975"/>
+          <a:off x="4667250" y="581025"/>
           <a:ext cx="6781800" cy="4619625"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -979,17 +1015,100 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:D21"/>
+  <dimension ref="A1:B8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G6" sqref="G6"/>
+      <selection activeCell="B2" sqref="B2:B8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="2" max="2" width="148.7109375" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2">
+      <c r="A1" t="s">
+        <v>94</v>
+      </c>
+      <c r="B1" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2">
+      <c r="A3">
+        <v>2</v>
+      </c>
+      <c r="B3" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2">
+      <c r="A4">
+        <v>3</v>
+      </c>
+      <c r="B4" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2">
+      <c r="A5">
+        <v>4</v>
+      </c>
+      <c r="B5" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2">
+      <c r="A6">
+        <v>5</v>
+      </c>
+      <c r="B6" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2">
+      <c r="A7">
+        <v>6</v>
+      </c>
+      <c r="B7" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2">
+      <c r="A8">
+        <v>7</v>
+      </c>
+      <c r="B8" t="s">
+        <v>101</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:D20"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="K32" sqref="K32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="33" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="29.7109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="3.5703125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="4.5703125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="21.42578125" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="78" bestFit="1" customWidth="1"/>
   </cols>
@@ -1051,7 +1170,10 @@
         <v>13</v>
       </c>
       <c r="B6" t="s">
-        <v>19</v>
+        <v>18</v>
+      </c>
+      <c r="C6" s="2" t="s">
+        <v>11</v>
       </c>
     </row>
     <row r="7" spans="1:4">
@@ -1059,7 +1181,10 @@
         <v>14</v>
       </c>
       <c r="B7" t="s">
-        <v>20</v>
+        <v>19</v>
+      </c>
+      <c r="C7" s="3" t="s">
+        <v>12</v>
       </c>
     </row>
     <row r="8" spans="1:4">
@@ -1067,7 +1192,10 @@
         <v>15</v>
       </c>
       <c r="B8" t="s">
-        <v>21</v>
+        <v>20</v>
+      </c>
+      <c r="C8" s="2" t="s">
+        <v>11</v>
       </c>
     </row>
     <row r="9" spans="1:4">
@@ -1077,6 +1205,9 @@
       <c r="B9" t="s">
         <v>4</v>
       </c>
+      <c r="C9" s="3" t="s">
+        <v>12</v>
+      </c>
     </row>
     <row r="10" spans="1:4">
       <c r="A10" t="s">
@@ -1085,21 +1216,27 @@
       <c r="B10" t="s">
         <v>4</v>
       </c>
+      <c r="C10" s="2" t="s">
+        <v>11</v>
+      </c>
     </row>
     <row r="11" spans="1:4">
       <c r="A11" t="s">
-        <v>18</v>
+        <v>22</v>
       </c>
       <c r="B11" t="s">
-        <v>4</v>
+        <v>21</v>
+      </c>
+      <c r="C11" s="3" t="s">
+        <v>12</v>
       </c>
     </row>
     <row r="12" spans="1:4">
       <c r="A12" t="s">
+        <v>22</v>
+      </c>
+      <c r="B12" t="s">
         <v>23</v>
-      </c>
-      <c r="B12" t="s">
-        <v>22</v>
       </c>
       <c r="C12" s="3" t="s">
         <v>12</v>
@@ -1107,48 +1244,45 @@
     </row>
     <row r="13" spans="1:4">
       <c r="A13" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="B13" t="s">
-        <v>24</v>
-      </c>
-      <c r="C13" s="3" t="s">
-        <v>12</v>
+        <v>25</v>
+      </c>
+      <c r="C13" s="2" t="s">
+        <v>11</v>
       </c>
     </row>
     <row r="14" spans="1:4">
       <c r="A14" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="B14" t="s">
-        <v>26</v>
-      </c>
-      <c r="C14" s="2" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="15" spans="1:4">
-      <c r="A15" t="s">
         <v>27</v>
       </c>
-      <c r="B15" t="s">
+      <c r="C14" s="3" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2">
+      <c r="A17" t="s">
         <v>28</v>
-      </c>
-      <c r="C15" s="3" t="s">
-        <v>12</v>
       </c>
     </row>
     <row r="18" spans="1:2">
       <c r="A18" t="s">
         <v>29</v>
       </c>
+      <c r="B18" t="s">
+        <v>2</v>
+      </c>
     </row>
     <row r="19" spans="1:2">
       <c r="A19" t="s">
         <v>30</v>
       </c>
       <c r="B19" t="s">
-        <v>2</v>
+        <v>32</v>
       </c>
     </row>
     <row r="20" spans="1:2">
@@ -1157,14 +1291,6 @@
       </c>
       <c r="B20" t="s">
         <v>33</v>
-      </c>
-    </row>
-    <row r="21" spans="1:2">
-      <c r="A21" t="s">
-        <v>32</v>
-      </c>
-      <c r="B21" t="s">
-        <v>34</v>
       </c>
     </row>
   </sheetData>
@@ -1174,7 +1300,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:C2"/>
   <sheetViews>
@@ -1190,18 +1316,18 @@
   <sheetData>
     <row r="1" spans="1:3">
       <c r="A1" t="s">
+        <v>34</v>
+      </c>
+      <c r="B1" t="s">
         <v>35</v>
       </c>
-      <c r="B1" t="s">
+      <c r="C1" t="s">
         <v>36</v>
-      </c>
-      <c r="C1" t="s">
-        <v>37</v>
       </c>
     </row>
     <row r="2" spans="1:3">
       <c r="A2" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B2" t="s">
         <v>0</v>
@@ -1216,12 +1342,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:E2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G1" sqref="G1"/>
+      <selection activeCell="B21" sqref="B21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1235,36 +1361,36 @@
   <sheetData>
     <row r="1" spans="1:5">
       <c r="A1" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C1" t="s">
+        <v>41</v>
+      </c>
+      <c r="D1" t="s">
+        <v>30</v>
+      </c>
+      <c r="E1" t="s">
         <v>42</v>
-      </c>
-      <c r="D1" t="s">
-        <v>31</v>
-      </c>
-      <c r="E1" t="s">
-        <v>43</v>
       </c>
     </row>
     <row r="2" spans="1:5">
       <c r="A2" t="s">
+        <v>39</v>
+      </c>
+      <c r="B2" t="s">
         <v>40</v>
-      </c>
-      <c r="B2" t="s">
-        <v>41</v>
       </c>
       <c r="C2" t="s">
         <v>2</v>
       </c>
       <c r="D2" t="s">
+        <v>32</v>
+      </c>
+      <c r="E2" t="s">
         <v>33</v>
-      </c>
-      <c r="E2" t="s">
-        <v>34</v>
       </c>
     </row>
   </sheetData>
@@ -1273,12 +1399,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:C2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B23" sqref="B23"/>
+      <selection activeCell="C23" sqref="C23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1292,21 +1418,21 @@
   <sheetData>
     <row r="1" spans="1:3">
       <c r="A1" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C1" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="2" spans="1:3">
       <c r="A2" t="s">
+        <v>39</v>
+      </c>
+      <c r="B2" t="s">
         <v>40</v>
-      </c>
-      <c r="B2" t="s">
-        <v>41</v>
       </c>
       <c r="C2" t="s">
         <v>2</v>
@@ -1318,12 +1444,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:C2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+      <selection activeCell="C27" sqref="C27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1334,228 +1460,24 @@
   <sheetData>
     <row r="1" spans="1:3">
       <c r="A1" t="s">
+        <v>54</v>
+      </c>
+      <c r="B1" t="s">
+        <v>35</v>
+      </c>
+      <c r="C1" t="s">
         <v>55</v>
-      </c>
-      <c r="B1" t="s">
-        <v>36</v>
-      </c>
-      <c r="C1" t="s">
-        <v>56</v>
       </c>
     </row>
     <row r="2" spans="1:3">
       <c r="A2" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B2" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C2" t="s">
-        <v>57</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <legacyDrawing r:id="rId1"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:D13"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
-  <cols>
-    <col min="1" max="1" width="77.5703125" customWidth="1"/>
-    <col min="2" max="2" width="33.42578125" bestFit="1" customWidth="1"/>
-    <col min="3" max="4" width="28.85546875" customWidth="1"/>
-    <col min="5" max="5" width="16.28515625" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:4">
-      <c r="A1" t="s">
-        <v>44</v>
-      </c>
-      <c r="B1" t="s">
-        <v>45</v>
-      </c>
-      <c r="C1" t="s">
-        <v>46</v>
-      </c>
-      <c r="D1" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4">
-      <c r="A2" t="s">
-        <v>48</v>
-      </c>
-      <c r="B2" t="s">
-        <v>41</v>
-      </c>
-      <c r="C2" t="s">
-        <v>60</v>
-      </c>
-      <c r="D2" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4">
-      <c r="A3" t="s">
-        <v>49</v>
-      </c>
-      <c r="B3" t="s">
-        <v>41</v>
-      </c>
-      <c r="C3" t="s">
-        <v>60</v>
-      </c>
-      <c r="D3" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4">
-      <c r="A4" t="s">
-        <v>66</v>
-      </c>
-      <c r="B4" t="s">
-        <v>41</v>
-      </c>
-      <c r="C4" t="s">
-        <v>61</v>
-      </c>
-      <c r="D4" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4">
-      <c r="A5" t="s">
-        <v>68</v>
-      </c>
-      <c r="B5" t="s">
-        <v>41</v>
-      </c>
-      <c r="C5" t="s">
-        <v>60</v>
-      </c>
-      <c r="D5" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4">
-      <c r="A6" t="s">
-        <v>50</v>
-      </c>
-      <c r="B6" t="s">
-        <v>41</v>
-      </c>
-      <c r="C6" t="s">
-        <v>60</v>
-      </c>
-      <c r="D6" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4">
-      <c r="A7" t="s">
-        <v>69</v>
-      </c>
-      <c r="B7" t="s">
-        <v>41</v>
-      </c>
-      <c r="C7" t="s">
-        <v>60</v>
-      </c>
-      <c r="D7" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4">
-      <c r="A8" t="s">
-        <v>70</v>
-      </c>
-      <c r="B8" t="s">
-        <v>41</v>
-      </c>
-      <c r="C8" t="s">
-        <v>60</v>
-      </c>
-      <c r="D8" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4">
-      <c r="A9" t="s">
-        <v>71</v>
-      </c>
-      <c r="B9" t="s">
-        <v>41</v>
-      </c>
-      <c r="C9" t="s">
-        <v>72</v>
-      </c>
-      <c r="D9" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4">
-      <c r="A10" t="s">
-        <v>51</v>
-      </c>
-      <c r="B10" t="s">
-        <v>41</v>
-      </c>
-      <c r="C10" t="s">
-        <v>60</v>
-      </c>
-      <c r="D10" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4">
-      <c r="A11" t="s">
-        <v>52</v>
-      </c>
-      <c r="B11" t="s">
-        <v>41</v>
-      </c>
-      <c r="C11" t="s">
-        <v>60</v>
-      </c>
-      <c r="D11" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4">
-      <c r="A12" t="s">
-        <v>53</v>
-      </c>
-      <c r="B12" t="s">
-        <v>41</v>
-      </c>
-      <c r="C12" t="s">
-        <v>72</v>
-      </c>
-      <c r="D12" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4">
-      <c r="A13" t="s">
-        <v>54</v>
-      </c>
-      <c r="B13" t="s">
-        <v>41</v>
-      </c>
-      <c r="C13" t="s">
-        <v>61</v>
-      </c>
-      <c r="D13" t="s">
-        <v>28</v>
+        <v>56</v>
       </c>
     </row>
   </sheetData>
@@ -1566,36 +1488,227 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:C20"/>
+  <dimension ref="A1:D12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C16" sqref="C16"/>
+      <selection activeCell="C23" sqref="C23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="83.5703125" customWidth="1"/>
+    <col min="1" max="1" width="77.5703125" customWidth="1"/>
+    <col min="2" max="2" width="33.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="22.28515625" customWidth="1"/>
+    <col min="4" max="4" width="28.85546875" customWidth="1"/>
+    <col min="5" max="5" width="16.28515625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4">
+      <c r="A1" t="s">
+        <v>43</v>
+      </c>
+      <c r="B1" t="s">
+        <v>44</v>
+      </c>
+      <c r="C1" t="s">
+        <v>45</v>
+      </c>
+      <c r="D1" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4">
+      <c r="A2" t="s">
+        <v>47</v>
+      </c>
+      <c r="B2" t="s">
+        <v>40</v>
+      </c>
+      <c r="C2" t="s">
+        <v>59</v>
+      </c>
+      <c r="D2" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4">
+      <c r="A3" t="s">
+        <v>48</v>
+      </c>
+      <c r="B3" t="s">
+        <v>40</v>
+      </c>
+      <c r="C3" t="s">
+        <v>59</v>
+      </c>
+      <c r="D3" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4">
+      <c r="A4" t="s">
+        <v>64</v>
+      </c>
+      <c r="B4" t="s">
+        <v>40</v>
+      </c>
+      <c r="C4" t="s">
+        <v>60</v>
+      </c>
+      <c r="D4" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4">
+      <c r="A5" t="s">
+        <v>66</v>
+      </c>
+      <c r="B5" t="s">
+        <v>40</v>
+      </c>
+      <c r="C5" t="s">
+        <v>59</v>
+      </c>
+      <c r="D5" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4">
+      <c r="A6" t="s">
+        <v>49</v>
+      </c>
+      <c r="B6" t="s">
+        <v>40</v>
+      </c>
+      <c r="C6" t="s">
+        <v>59</v>
+      </c>
+      <c r="D6" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4">
+      <c r="A7" t="s">
+        <v>67</v>
+      </c>
+      <c r="B7" t="s">
+        <v>40</v>
+      </c>
+      <c r="C7" t="s">
+        <v>59</v>
+      </c>
+      <c r="D7" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4">
+      <c r="A8" t="s">
+        <v>68</v>
+      </c>
+      <c r="B8" t="s">
+        <v>40</v>
+      </c>
+      <c r="C8" t="s">
+        <v>69</v>
+      </c>
+      <c r="D8" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4">
+      <c r="A9" t="s">
+        <v>50</v>
+      </c>
+      <c r="B9" t="s">
+        <v>40</v>
+      </c>
+      <c r="C9" t="s">
+        <v>59</v>
+      </c>
+      <c r="D9" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4">
+      <c r="A10" t="s">
+        <v>51</v>
+      </c>
+      <c r="B10" t="s">
+        <v>40</v>
+      </c>
+      <c r="C10" t="s">
+        <v>59</v>
+      </c>
+      <c r="D10" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4">
+      <c r="A11" t="s">
+        <v>52</v>
+      </c>
+      <c r="B11" t="s">
+        <v>40</v>
+      </c>
+      <c r="C11" t="s">
+        <v>69</v>
+      </c>
+      <c r="D11" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4">
+      <c r="A12" t="s">
+        <v>53</v>
+      </c>
+      <c r="B12" t="s">
+        <v>40</v>
+      </c>
+      <c r="C12" t="s">
+        <v>60</v>
+      </c>
+      <c r="D12" t="s">
+        <v>27</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <legacyDrawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:C19"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A27" sqref="A27"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="76.28515625" customWidth="1"/>
     <col min="2" max="2" width="50" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="45.140625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3">
       <c r="A1" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="B1" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="C1" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
     </row>
     <row r="2" spans="1:3">
       <c r="A2" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
       <c r="B2" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="C2" s="3" t="s">
         <v>12</v>
@@ -1603,10 +1716,10 @@
     </row>
     <row r="3" spans="1:3">
       <c r="A3" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
       <c r="B3" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="C3" s="3" t="s">
         <v>12</v>
@@ -1614,10 +1727,10 @@
     </row>
     <row r="4" spans="1:3">
       <c r="A4" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
       <c r="B4" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="C4" s="2" t="s">
         <v>11</v>
@@ -1625,10 +1738,10 @@
     </row>
     <row r="5" spans="1:3">
       <c r="A5" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
       <c r="B5" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="C5" s="2" t="s">
         <v>11</v>
@@ -1636,10 +1749,10 @@
     </row>
     <row r="6" spans="1:3">
       <c r="A6" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
       <c r="B6" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="C6" s="2" t="s">
         <v>11</v>
@@ -1647,10 +1760,10 @@
     </row>
     <row r="7" spans="1:3">
       <c r="A7" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
       <c r="B7" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="C7" s="2" t="s">
         <v>11</v>
@@ -1658,10 +1771,10 @@
     </row>
     <row r="8" spans="1:3">
       <c r="A8" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="B8" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="C8" s="2" t="s">
         <v>11</v>
@@ -1669,21 +1782,21 @@
     </row>
     <row r="9" spans="1:3">
       <c r="A9" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="B9" t="s">
-        <v>76</v>
-      </c>
-      <c r="C9" s="2" t="s">
-        <v>11</v>
+        <v>73</v>
+      </c>
+      <c r="C9" s="3" t="s">
+        <v>12</v>
       </c>
     </row>
     <row r="10" spans="1:3">
       <c r="A10" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="B10" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="C10" s="3" t="s">
         <v>12</v>
@@ -1691,112 +1804,101 @@
     </row>
     <row r="11" spans="1:3">
       <c r="A11" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="B11" t="s">
-        <v>76</v>
-      </c>
-      <c r="C11" s="3" t="s">
-        <v>12</v>
+        <v>73</v>
+      </c>
+      <c r="C11" s="2" t="s">
+        <v>11</v>
       </c>
     </row>
     <row r="12" spans="1:3">
       <c r="A12" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="B12" t="s">
-        <v>76</v>
-      </c>
-      <c r="C12" s="2" t="s">
-        <v>11</v>
+        <v>73</v>
+      </c>
+      <c r="C12" s="3" t="s">
+        <v>12</v>
       </c>
     </row>
     <row r="13" spans="1:3">
       <c r="A13" t="s">
-        <v>96</v>
+        <v>82</v>
       </c>
       <c r="B13" t="s">
-        <v>76</v>
-      </c>
-      <c r="C13" s="3" t="s">
-        <v>12</v>
+        <v>74</v>
+      </c>
+      <c r="C13" t="s">
+        <v>81</v>
       </c>
     </row>
     <row r="14" spans="1:3">
       <c r="A14" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="B14" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="C14" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
     </row>
     <row r="15" spans="1:3">
       <c r="A15" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="B15" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="C15" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
     </row>
     <row r="16" spans="1:3">
       <c r="A16" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="B16" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="C16" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
     </row>
     <row r="17" spans="1:3">
       <c r="A17" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="B17" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="C17" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
     </row>
     <row r="18" spans="1:3">
       <c r="A18" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="B18" t="s">
+        <v>79</v>
+      </c>
+      <c r="C18" t="s">
         <v>81</v>
-      </c>
-      <c r="C18" t="s">
-        <v>84</v>
       </c>
     </row>
     <row r="19" spans="1:3">
       <c r="A19" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="B19" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="C19" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="20" spans="1:3">
-      <c r="A20" t="s">
-        <v>94</v>
-      </c>
-      <c r="B20" t="s">
-        <v>83</v>
-      </c>
-      <c r="C20" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Cleaning up to be FHIM "spec" spreadsheet.
</commit_message>
<xml_diff>
--- a/resources/FHIM_dbp_refSetMapping.xlsx
+++ b/resources/FHIM_dbp_refSetMapping.xlsx
@@ -1,22 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" tabRatio="758"/>
+    <workbookView xWindow="240" yWindow="108" windowWidth="14808" windowHeight="8016" tabRatio="758"/>
   </bookViews>
   <sheets>
-    <sheet name="Questions" sheetId="8" r:id="rId1"/>
-    <sheet name="source" sheetId="1" r:id="rId2"/>
-    <sheet name="FHIMObservationRefSet" sheetId="2" r:id="rId3"/>
-    <sheet name="FHIMObservationCodeRefSet" sheetId="3" r:id="rId4"/>
-    <sheet name="AltFHIMObservationCodeRefSet" sheetId="6" r:id="rId5"/>
-    <sheet name="FHIMObservationDataRefSet" sheetId="5" r:id="rId6"/>
-    <sheet name="FHIMObservationCompRefSet" sheetId="4" r:id="rId7"/>
-    <sheet name="FHIMObservationConstraintRefSet" sheetId="7" r:id="rId8"/>
+    <sheet name="source" sheetId="1" r:id="rId1"/>
+    <sheet name="FHIMObservationRefSet" sheetId="2" r:id="rId2"/>
+    <sheet name="AltFHIMObservationCodeRefSet" sheetId="6" r:id="rId3"/>
+    <sheet name="FHIMObservationDataRefSet" sheetId="5" r:id="rId4"/>
+    <sheet name="FHIMObservationCompRefSet" sheetId="4" r:id="rId5"/>
+    <sheet name="FHIMObservationConstraintRefSet" sheetId="7" r:id="rId6"/>
   </sheets>
-  <calcPr calcId="125725" concurrentCalc="0"/>
+  <calcPr calcId="152511" concurrentCalc="0"/>
 </workbook>
 </file>
 
@@ -26,7 +24,7 @@
     <author>Author</author>
   </authors>
   <commentList>
-    <comment ref="B2" authorId="0">
+    <comment ref="B2" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -50,7 +48,7 @@
     <author>Author</author>
   </authors>
   <commentList>
-    <comment ref="B2" authorId="0">
+    <comment ref="B2" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -74,7 +72,7 @@
     <author>Author</author>
   </authors>
   <commentList>
-    <comment ref="B2" authorId="0">
+    <comment ref="B2" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -98,7 +96,7 @@
     <author>Author</author>
   </authors>
   <commentList>
-    <comment ref="B2" authorId="0">
+    <comment ref="B2" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -112,17 +110,7 @@
         </r>
       </text>
     </comment>
-  </commentList>
-</comments>
-</file>
-
-<file path=xl/comments5.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <authors>
-    <author>Author</author>
-  </authors>
-  <commentList>
-    <comment ref="B2" authorId="0">
+    <comment ref="B3" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -136,7 +124,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="B3" authorId="0">
+    <comment ref="B4" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -150,7 +138,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="B4" authorId="0">
+    <comment ref="B5" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -164,7 +152,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="B5" authorId="0">
+    <comment ref="B6" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -178,7 +166,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="B6" authorId="0">
+    <comment ref="B7" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -192,7 +180,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="B7" authorId="0">
+    <comment ref="B8" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -206,7 +194,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="B8" authorId="0">
+    <comment ref="B9" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -220,7 +208,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="B9" authorId="0">
+    <comment ref="B10" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -234,7 +222,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="B10" authorId="0">
+    <comment ref="B11" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -248,21 +236,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="B11" authorId="0">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>temporarily using name, but will be an SCT CID</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="B12" authorId="0">
+    <comment ref="B12" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -281,7 +255,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="190" uniqueCount="103">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="169" uniqueCount="92">
   <si>
     <t>DiastolicBloodPressureObservation</t>
   </si>
@@ -406,12 +380,6 @@
     <t xml:space="preserve">DiastolicBloodPressureObservation </t>
   </si>
   <si>
-    <t>code (string)</t>
-  </si>
-  <si>
-    <t>codeDisplayText</t>
-  </si>
-  <si>
     <t>memberID (CID)</t>
   </si>
   <si>
@@ -505,30 +473,6 @@
     <t>card</t>
   </si>
   <si>
-    <t>qual.BloodPressureBodySitedata.cwe.domain</t>
-  </si>
-  <si>
-    <t>qual.BloodPressureMethoddata.cwe.domain</t>
-  </si>
-  <si>
-    <t>qual.Reliabilitydata.cwe.domain</t>
-  </si>
-  <si>
-    <t>qual.Severitydata.cwe.domain</t>
-  </si>
-  <si>
-    <t>qual.Statusdata.cwe.domain</t>
-  </si>
-  <si>
-    <t>qual.BloodPressureCuffSizeQualifierdata.cwe.domain</t>
-  </si>
-  <si>
-    <t>qual.BloodPressurePositionQualifierdata.cwe.domain</t>
-  </si>
-  <si>
-    <t>[OID tbd]</t>
-  </si>
-  <si>
     <t>componentId for BloodPressureBodySite in FHIMObservationComposition</t>
   </si>
   <si>
@@ -547,9 +491,6 @@
     <t>componentId for Reliability in FHIMObservationComposition</t>
   </si>
   <si>
-    <t>componentId for Severity in FHIMObservationComposition</t>
-  </si>
-  <si>
     <t>componentId for Status in FHIMObservationComposition</t>
   </si>
   <si>
@@ -565,61 +506,38 @@
     <t>componentId for Provenance in FHIMObservationComposition</t>
   </si>
   <si>
-    <t>#</t>
-  </si>
-  <si>
-    <t>Are there any criteria for refset type selection--i.e., whether to include more columns in fewer refsets or fewer columns in more refsets?</t>
-  </si>
-  <si>
-    <t>In the base model refset, a concept ID is associated with a type. Why is this? Is it in order to differentiate different model types (FHIM, CEM) for the same concept?</t>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">In the CEM key refset, an IMHC key code is associated with the concept identifier. Wouldn't that key code </t>
-    </r>
-    <r>
-      <rPr>
-        <u/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>be</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> the concept identifier?</t>
-    </r>
-  </si>
-  <si>
-    <t>In the FHIM key refset, should the LOINC code be a CID, assuming it's in the workbench environment, or do we need to specify its system and text?</t>
-  </si>
-  <si>
-    <t>Do we want to classify components as CEM does, if the source model does not?</t>
-  </si>
-  <si>
-    <t>Constraints use a property called "path," which seems to be a description of the kind of constraint, but which I'd expect to be a concept rather than a string.</t>
-  </si>
-  <si>
-    <t>I've asserted some constraint criteria as value set OIDs. Does that fit in this conceptual solution?</t>
-  </si>
-  <si>
-    <t>Question</t>
+    <t>qual.bloodPressureBodySite.data.cwe.domain</t>
+  </si>
+  <si>
+    <t>qual.bloodPressureMethod.data.cwe.domain</t>
+  </si>
+  <si>
+    <t>qual.reliability.data.cwe.domain</t>
+  </si>
+  <si>
+    <t>qual.status.data.cwe.domain</t>
+  </si>
+  <si>
+    <t>qual.bloodPressureCuffSizeQualifier.data.cwe.domain</t>
+  </si>
+  <si>
+    <t>qual.bloodPressurePositionQualifier.data.cwe.domain</t>
+  </si>
+  <si>
+    <t>cs=LOINC, c=8462-4</t>
+  </si>
+  <si>
+    <t>componentID for DiastolicBloodPressureMeas</t>
+  </si>
+  <si>
+    <t>codeSystemVersion</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="4">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -642,14 +560,6 @@
       <name val="Tahoma"/>
       <family val="2"/>
     </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -671,17 +581,29 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="20" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -773,7 +695,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -805,9 +727,10 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -839,6 +762,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -1014,111 +938,28 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:B8"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:D21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2:B8"/>
+      <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
-  <cols>
-    <col min="2" max="2" width="148.7109375" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:2">
-      <c r="A1" t="s">
-        <v>94</v>
-      </c>
-      <c r="B1" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2">
-      <c r="A2">
-        <v>1</v>
-      </c>
-      <c r="B2" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2">
-      <c r="A3">
-        <v>2</v>
-      </c>
-      <c r="B3" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2">
-      <c r="A4">
-        <v>3</v>
-      </c>
-      <c r="B4" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2">
-      <c r="A5">
-        <v>4</v>
-      </c>
-      <c r="B5" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2">
-      <c r="A6">
-        <v>5</v>
-      </c>
-      <c r="B6" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2">
-      <c r="A7">
-        <v>6</v>
-      </c>
-      <c r="B7" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2">
-      <c r="A8">
-        <v>7</v>
-      </c>
-      <c r="B8" t="s">
-        <v>101</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:D20"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="K32" sqref="K32"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="33" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="29.7109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="4.5703125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="21.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="29.6640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="4.5546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="21.44140625" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="78" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:4">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>1</v>
       </c>
@@ -1132,7 +973,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:4">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>6</v>
       </c>
@@ -1143,7 +984,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="4" spans="1:4">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>7</v>
       </c>
@@ -1154,7 +995,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="5" spans="1:4">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>8</v>
       </c>
@@ -1165,7 +1006,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="6" spans="1:4">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>13</v>
       </c>
@@ -1176,7 +1017,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="7" spans="1:4">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>14</v>
       </c>
@@ -1187,7 +1028,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="8" spans="1:4">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>15</v>
       </c>
@@ -1198,7 +1039,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="9" spans="1:4">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>16</v>
       </c>
@@ -1209,7 +1050,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="10" spans="1:4">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>17</v>
       </c>
@@ -1220,7 +1061,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="11" spans="1:4">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>22</v>
       </c>
@@ -1231,7 +1072,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="12" spans="1:4">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>22</v>
       </c>
@@ -1242,7 +1083,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="13" spans="1:4">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>24</v>
       </c>
@@ -1253,7 +1094,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="14" spans="1:4">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>26</v>
       </c>
@@ -1264,12 +1105,12 @@
         <v>12</v>
       </c>
     </row>
-    <row r="17" spans="1:2">
+    <row r="17" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="18" spans="1:2">
+    <row r="18" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>29</v>
       </c>
@@ -1277,7 +1118,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="19" spans="1:2">
+    <row r="19" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>30</v>
       </c>
@@ -1285,12 +1126,20 @@
         <v>32</v>
       </c>
     </row>
-    <row r="20" spans="1:2">
+    <row r="20" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
         <v>31</v>
       </c>
       <c r="B20" t="s">
         <v>33</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A21" t="s">
+        <v>91</v>
+      </c>
+      <c r="B21" s="4">
+        <v>2.42</v>
       </c>
     </row>
   </sheetData>
@@ -1300,21 +1149,21 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="51.140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="51.109375" bestFit="1" customWidth="1"/>
     <col min="2" max="3" width="33" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>34</v>
       </c>
@@ -1325,7 +1174,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="2" spans="1:3">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>37</v>
       </c>
@@ -1334,6 +1183,51 @@
       </c>
       <c r="C2" t="s">
         <v>0</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <legacyDrawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:C2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C2" sqref="C2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="51.109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="37.6640625" customWidth="1"/>
+    <col min="3" max="3" width="17.5546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11.6640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="22.6640625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>34</v>
+      </c>
+      <c r="B1" t="s">
+        <v>38</v>
+      </c>
+      <c r="C1" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>39</v>
+      </c>
+      <c r="B2" t="s">
+        <v>40</v>
+      </c>
+      <c r="C2" t="s">
+        <v>89</v>
       </c>
     </row>
   </sheetData>
@@ -1343,54 +1237,39 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:E2"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:C2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B21" sqref="B21"/>
+      <selection activeCell="C27" sqref="C27"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="51.140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="37.7109375" customWidth="1"/>
-    <col min="3" max="3" width="12.140625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="11.7109375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="22.7109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="76.44140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="3" width="33" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>34</v>
+        <v>52</v>
       </c>
       <c r="B1" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="C1" t="s">
-        <v>41</v>
-      </c>
-      <c r="D1" t="s">
-        <v>30</v>
-      </c>
-      <c r="E1" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>39</v>
+        <v>55</v>
       </c>
       <c r="B2" t="s">
         <v>40</v>
       </c>
       <c r="C2" t="s">
-        <v>2</v>
-      </c>
-      <c r="D2" t="s">
-        <v>32</v>
-      </c>
-      <c r="E2" t="s">
-        <v>33</v>
+        <v>54</v>
       </c>
     </row>
   </sheetData>
@@ -1400,42 +1279,188 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:C2"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:D12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C23" sqref="C23"/>
+      <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="51.140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="37.7109375" customWidth="1"/>
-    <col min="3" max="3" width="12.140625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="11.7109375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="22.7109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="77.5546875" customWidth="1"/>
+    <col min="2" max="2" width="33.44140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="22.33203125" customWidth="1"/>
+    <col min="4" max="4" width="28.88671875" customWidth="1"/>
+    <col min="5" max="5" width="16.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>34</v>
+        <v>41</v>
       </c>
       <c r="B1" t="s">
-        <v>38</v>
+        <v>42</v>
       </c>
       <c r="C1" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3">
+        <v>43</v>
+      </c>
+      <c r="D1" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>39</v>
+        <v>45</v>
       </c>
       <c r="B2" t="s">
         <v>40</v>
       </c>
       <c r="C2" t="s">
-        <v>2</v>
+        <v>57</v>
+      </c>
+      <c r="D2" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>46</v>
+      </c>
+      <c r="B3" t="s">
+        <v>40</v>
+      </c>
+      <c r="C3" t="s">
+        <v>57</v>
+      </c>
+      <c r="D3" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>62</v>
+      </c>
+      <c r="B4" t="s">
+        <v>40</v>
+      </c>
+      <c r="C4" t="s">
+        <v>58</v>
+      </c>
+      <c r="D4" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>64</v>
+      </c>
+      <c r="B5" t="s">
+        <v>40</v>
+      </c>
+      <c r="C5" t="s">
+        <v>57</v>
+      </c>
+      <c r="D5" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>47</v>
+      </c>
+      <c r="B6" t="s">
+        <v>40</v>
+      </c>
+      <c r="C6" t="s">
+        <v>57</v>
+      </c>
+      <c r="D6" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
+        <v>65</v>
+      </c>
+      <c r="B7" t="s">
+        <v>40</v>
+      </c>
+      <c r="C7" t="s">
+        <v>57</v>
+      </c>
+      <c r="D7" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A8" t="s">
+        <v>66</v>
+      </c>
+      <c r="B8" t="s">
+        <v>40</v>
+      </c>
+      <c r="C8" t="s">
+        <v>67</v>
+      </c>
+      <c r="D8" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A9" t="s">
+        <v>48</v>
+      </c>
+      <c r="B9" t="s">
+        <v>40</v>
+      </c>
+      <c r="C9" t="s">
+        <v>57</v>
+      </c>
+      <c r="D9" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A10" t="s">
+        <v>49</v>
+      </c>
+      <c r="B10" t="s">
+        <v>40</v>
+      </c>
+      <c r="C10" t="s">
+        <v>57</v>
+      </c>
+      <c r="D10" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A11" t="s">
+        <v>50</v>
+      </c>
+      <c r="B11" t="s">
+        <v>40</v>
+      </c>
+      <c r="C11" t="s">
+        <v>67</v>
+      </c>
+      <c r="D11" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A12" t="s">
+        <v>51</v>
+      </c>
+      <c r="B12" t="s">
+        <v>40</v>
+      </c>
+      <c r="C12" t="s">
+        <v>58</v>
+      </c>
+      <c r="D12" t="s">
+        <v>27</v>
       </c>
     </row>
   </sheetData>
@@ -1445,460 +1470,216 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:C2"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:C18"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C27" sqref="C27"/>
+      <selection activeCell="A21" sqref="A21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="76.42578125" bestFit="1" customWidth="1"/>
-    <col min="2" max="3" width="33" customWidth="1"/>
+    <col min="1" max="1" width="76.33203125" customWidth="1"/>
+    <col min="2" max="2" width="50" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="45.109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>54</v>
+        <v>68</v>
       </c>
       <c r="B1" t="s">
-        <v>35</v>
+        <v>69</v>
       </c>
       <c r="C1" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>57</v>
+        <v>72</v>
       </c>
       <c r="B2" t="s">
-        <v>40</v>
-      </c>
-      <c r="C2" t="s">
-        <v>56</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <legacyDrawing r:id="rId1"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:D12"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C23" sqref="C23"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
-  <cols>
-    <col min="1" max="1" width="77.5703125" customWidth="1"/>
-    <col min="2" max="2" width="33.42578125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="22.28515625" customWidth="1"/>
-    <col min="4" max="4" width="28.85546875" customWidth="1"/>
-    <col min="5" max="5" width="16.28515625" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:4">
-      <c r="A1" t="s">
-        <v>43</v>
-      </c>
-      <c r="B1" t="s">
-        <v>44</v>
-      </c>
-      <c r="C1" t="s">
-        <v>45</v>
-      </c>
-      <c r="D1" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4">
-      <c r="A2" t="s">
-        <v>47</v>
-      </c>
-      <c r="B2" t="s">
-        <v>40</v>
-      </c>
-      <c r="C2" t="s">
-        <v>59</v>
-      </c>
-      <c r="D2" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4">
-      <c r="A3" t="s">
-        <v>48</v>
-      </c>
-      <c r="B3" t="s">
-        <v>40</v>
-      </c>
-      <c r="C3" t="s">
-        <v>59</v>
-      </c>
-      <c r="D3" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4">
-      <c r="A4" t="s">
-        <v>64</v>
-      </c>
-      <c r="B4" t="s">
-        <v>40</v>
-      </c>
-      <c r="C4" t="s">
-        <v>60</v>
-      </c>
-      <c r="D4" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4">
-      <c r="A5" t="s">
-        <v>66</v>
-      </c>
-      <c r="B5" t="s">
-        <v>40</v>
-      </c>
-      <c r="C5" t="s">
-        <v>59</v>
-      </c>
-      <c r="D5" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4">
-      <c r="A6" t="s">
-        <v>49</v>
-      </c>
-      <c r="B6" t="s">
-        <v>40</v>
-      </c>
-      <c r="C6" t="s">
-        <v>59</v>
-      </c>
-      <c r="D6" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4">
-      <c r="A7" t="s">
-        <v>67</v>
-      </c>
-      <c r="B7" t="s">
-        <v>40</v>
-      </c>
-      <c r="C7" t="s">
-        <v>59</v>
-      </c>
-      <c r="D7" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4">
-      <c r="A8" t="s">
-        <v>68</v>
-      </c>
-      <c r="B8" t="s">
-        <v>40</v>
-      </c>
-      <c r="C8" t="s">
-        <v>69</v>
-      </c>
-      <c r="D8" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4">
-      <c r="A9" t="s">
-        <v>50</v>
-      </c>
-      <c r="B9" t="s">
-        <v>40</v>
-      </c>
-      <c r="C9" t="s">
-        <v>59</v>
-      </c>
-      <c r="D9" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4">
-      <c r="A10" t="s">
-        <v>51</v>
-      </c>
-      <c r="B10" t="s">
-        <v>40</v>
-      </c>
-      <c r="C10" t="s">
-        <v>59</v>
-      </c>
-      <c r="D10" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4">
-      <c r="A11" t="s">
-        <v>52</v>
-      </c>
-      <c r="B11" t="s">
-        <v>40</v>
-      </c>
-      <c r="C11" t="s">
-        <v>69</v>
-      </c>
-      <c r="D11" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4">
-      <c r="A12" t="s">
-        <v>53</v>
-      </c>
-      <c r="B12" t="s">
-        <v>40</v>
-      </c>
-      <c r="C12" t="s">
-        <v>60</v>
-      </c>
-      <c r="D12" t="s">
-        <v>27</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <legacyDrawing r:id="rId1"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:C19"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A27" sqref="A27"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
-  <cols>
-    <col min="1" max="1" width="76.28515625" customWidth="1"/>
-    <col min="2" max="2" width="50" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="45.140625" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:3">
-      <c r="A1" t="s">
-        <v>70</v>
-      </c>
-      <c r="B1" t="s">
         <v>71</v>
-      </c>
-      <c r="C1" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3">
-      <c r="A2" t="s">
-        <v>82</v>
-      </c>
-      <c r="B2" t="s">
-        <v>73</v>
       </c>
       <c r="C2" s="3" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="3" spans="1:3">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>83</v>
+        <v>73</v>
       </c>
       <c r="B3" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="C3" s="3" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="4" spans="1:3">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>84</v>
+        <v>74</v>
       </c>
       <c r="B4" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="C4" s="2" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="5" spans="1:3">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>85</v>
+        <v>75</v>
       </c>
       <c r="B5" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="C5" s="2" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="6" spans="1:3">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>86</v>
+        <v>76</v>
       </c>
       <c r="B6" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="C6" s="2" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="7" spans="1:3">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>87</v>
+        <v>77</v>
       </c>
       <c r="B7" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="C7" s="2" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="8" spans="1:3">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>89</v>
+        <v>78</v>
       </c>
       <c r="B8" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="C8" s="2" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="9" spans="1:3">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>90</v>
+        <v>79</v>
       </c>
       <c r="B9" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="C9" s="3" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="10" spans="1:3">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>91</v>
+        <v>80</v>
       </c>
       <c r="B10" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="C10" s="3" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="11" spans="1:3">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>92</v>
+        <v>81</v>
       </c>
       <c r="B11" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="C11" s="2" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="12" spans="1:3">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
-        <v>93</v>
+        <v>82</v>
       </c>
       <c r="B12" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="C12" s="3" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="13" spans="1:3">
-      <c r="A13" t="s">
-        <v>82</v>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A13" s="5" t="s">
+        <v>90</v>
       </c>
       <c r="B13" t="s">
-        <v>74</v>
+        <v>83</v>
       </c>
       <c r="C13" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="14" spans="1:3">
-      <c r="A14" t="s">
-        <v>83</v>
+        <v>9</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A14" s="5" t="s">
+        <v>90</v>
       </c>
       <c r="B14" t="s">
-        <v>75</v>
+        <v>84</v>
       </c>
       <c r="C14" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="15" spans="1:3">
-      <c r="A15" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A15" s="5" t="s">
+        <v>90</v>
+      </c>
+      <c r="B15" t="s">
+        <v>85</v>
+      </c>
+      <c r="C15" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A16" s="5" t="s">
+        <v>90</v>
+      </c>
+      <c r="B16" t="s">
+        <v>86</v>
+      </c>
+      <c r="C16" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A17" s="5" t="s">
+        <v>90</v>
+      </c>
+      <c r="B17" t="s">
         <v>87</v>
       </c>
-      <c r="B15" t="s">
-        <v>76</v>
-      </c>
-      <c r="C15" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="16" spans="1:3">
-      <c r="A16" t="s">
+      <c r="C17" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A18" s="5" t="s">
+        <v>90</v>
+      </c>
+      <c r="B18" t="s">
         <v>88</v>
       </c>
-      <c r="B16" t="s">
-        <v>77</v>
-      </c>
-      <c r="C16" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="17" spans="1:3">
-      <c r="A17" t="s">
-        <v>89</v>
-      </c>
-      <c r="B17" t="s">
-        <v>78</v>
-      </c>
-      <c r="C17" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="18" spans="1:3">
-      <c r="A18" t="s">
-        <v>90</v>
-      </c>
-      <c r="B18" t="s">
-        <v>79</v>
-      </c>
       <c r="C18" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="19" spans="1:3">
-      <c r="A19" t="s">
-        <v>91</v>
-      </c>
-      <c r="B19" t="s">
-        <v>80</v>
-      </c>
-      <c r="C19" t="s">
-        <v>81</v>
+        <v>23</v>
       </c>
     </row>
   </sheetData>

</xml_diff>